<commit_message>
cập nhật tài liệu
+lịch trình
+đặc tả yêu cầu
+cập nhật kế hoạch
</commit_message>
<xml_diff>
--- a/docs/phân chia công việc.xlsx
+++ b/docs/phân chia công việc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\GitSource\QuanLyNhaSach\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BF5FC646-17C4-4BB2-B8DF-64A48EC30DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB08BD35-3A50-41B6-925C-E35AB8A8B35E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>LẬP DANH SÁCH 10 THÀNH VIÊN &amp; PHÂN VAI</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>Tester – Kiểm thử</t>
-  </si>
-  <si>
-    <t>Deployment – Triển khai</t>
   </si>
   <si>
     <t>Khanh</t>
@@ -147,7 +144,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -170,11 +167,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -187,7 +223,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -470,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -501,33 +555,29 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="5">
+      <c r="A4" s="11">
         <v>1</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>12</v>
+      <c r="B4" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="5">
-        <v>2</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="A5" s="12"/>
+      <c r="B5" s="7"/>
       <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>6</v>
@@ -535,10 +585,10 @@
     </row>
     <row r="7" spans="1:3" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>7</v>
@@ -546,21 +596,21 @@
     </row>
     <row r="8" spans="1:3" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>8</v>
@@ -568,21 +618,21 @@
     </row>
     <row r="10" spans="1:3" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>9</v>
@@ -590,38 +640,45 @@
     </row>
     <row r="12" spans="1:3" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
+        <v>8</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
+        <v>9</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="5" t="s">
+    </row>
+    <row r="14" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="5">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="1">
-        <v>11</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="B14" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="24.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C15" s="9"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>